<commit_message>
add new reimburse data
</commit_message>
<xml_diff>
--- a/莆田项目部公共开支明细表数据库版本20170421起.xlsx
+++ b/莆田项目部公共开支明细表数据库版本20170421起.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="逐日消费统计表" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,6 +204,34 @@
   </si>
   <si>
     <t>莆田</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林迪南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林迪南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郑景祥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伙食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公交车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伙食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吴紫东</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -559,9 +587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -643,6 +673,24 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>20170511</v>
+      </c>
+      <c r="C5">
+        <f>3+35+100+4+51+5</f>
+        <v>198</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -652,10 +700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -712,6 +760,20 @@
         <v>72.3</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20170511</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="4">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -721,10 +783,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -791,6 +853,77 @@
         <v>40</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20170511</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1">
+        <f>100/3+51/2</f>
+        <v>58.833333333333336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20170511</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20170511</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="1">
+        <f>100/3+51/2+4</f>
+        <v>62.833333333333336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20170511</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1">
+        <f>100/3</f>
+        <v>33.333333333333336</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -800,10 +933,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -927,6 +1060,42 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>20170511</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>20170511</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>20170511</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -939,7 +1108,7 @@
   <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1020,9 +1189,33 @@
         <v>29</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>20170511</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>20170511</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="6"/>
@@ -1346,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1416,6 +1609,28 @@
       </c>
       <c r="C5">
         <v>20170510</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>20170511</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>20170511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>